<commit_message>
new trait extraction and new field sheet
</commit_message>
<xml_diff>
--- a/Manual_trait_extraction/Fagales fill-in_controlled_fields.xlsx
+++ b/Manual_trait_extraction/Fagales fill-in_controlled_fields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryanfolk/Documents/GitHub/fagales_traits/Manual_trait_extraction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B3556-67AF-DB45-A963-87C260538351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374E1A45-B93C-484F-9286-D158FAED9066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="800" yWindow="520" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="5120" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2379,10 +2379,10 @@
   <dimension ref="A1:AW215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F119" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L140" sqref="L140"/>
+      <selection pane="bottomRight" activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>